<commit_message>
- Config 파일 설정   • Name: RPA10_경기도뉴스포털_RE_노유정   • Website Info: https://gnews.gg.go.kr/briefing/brief_gongbo.do   • Output 폴더 및 Today (yyyyMMdd) 설정   • 메일 제목 및 본문 포맷 템플릿화
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sma06\Desktop\RPAWorkspace\RE-Framework 템플릿\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yache\Desktop\RPAWorkspace\RPA10_경기도뉴스포털_RE_노유정\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EE182E-F582-4CA8-8E45-48862A7AED08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414709CC-B606-4B2F-BB71-ECF65782F6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -123,15 +123,6 @@
   </si>
   <si>
     <t>MailBody</t>
-  </si>
-  <si>
-    <t>{0}=날짜
-{1}=과제명 dicConfig("과제명").ToString
-{2}=결과시트 링크
-{3}=intTotalCnt
-{4}=intSuccessCnt
-{5}=intFailCnt
-{6}=strMemo</t>
   </si>
   <si>
     <t>MailBody_NoData</t>
@@ -316,10 +307,6 @@
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>RE-Framework 템플릿</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>기준정보SheetId</t>
@@ -402,16 +389,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>[RPA_{0}] {1} 처리 결과 : {2}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}=부서코드
-{1}=과제명 dicConfig("과제명").ToString
-{2}= 성공입니다. &amp; 실패입니다. &amp; 처리할 Data가 없습니다.</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Temp.xlsx</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -455,10 +432,6 @@
     <t>MailTo2</t>
   </si>
   <si>
-    <t>본인 메일</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>minasong621@gmail.com</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -544,13 +517,24 @@
     <r>
       <rPr>
         <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{2}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <color rgb="FF00B050"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>결과 데이터를</t>
+      <t>를</t>
     </r>
     <r>
       <rPr>
@@ -609,143 +593,81 @@
     <r>
       <rPr>
         <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Link : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <color rgb="FFFF0000"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{2}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;/span&gt;&lt;/p&gt;
-&lt;table cellspacing="0" cellpadding="0" border="1" style="width: 776px; height: 60px; font-size: 10pt; border-width: 0px; border-color: rgb(0, 0, 0); border-collapse: collapse; border-style: solid; background-color: rgb(255, 255, 255); background-image: none; background-repeat: repeat; background-position: 0% 0%;" class=""&gt;
-&lt;tbody&gt;
-&lt;tr&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>총건수</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>처리건수</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" colspan="1" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>미처리건수</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" colspan="1" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>비</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp; &amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>고</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;/tr&gt;
-&lt;tr&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+      <t>{3}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Today</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>yyyyMMdd 형식</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>yacheku@gmail.com</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>RPA10_경기도뉴스포털_RE_노유정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutputFolder</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>OutputPath</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Data\Output</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://gnews.gg.go.kr/briefing/brief_gongbo.do</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>{0} 첨부파일에 hwpx 파일 부재 알립니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}=yyyyMMdd(오늘날짜)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;안녕하세요.&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
     </r>
     <r>
       <rPr>
@@ -756,19 +678,18 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{3}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt; color: rgb(0, 0, 255); font-weight: bold;"&gt;</t>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~</t>
     </r>
     <r>
       <rPr>
@@ -779,134 +700,18 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{4}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;" colspan="1"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0); font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{5}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;" colspan="1"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{6}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;/tr&gt;</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RPA_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>결과 안내 메일입니다.</t>
+      <t xml:space="preserve"> {1} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>검색기간내에 hwpx 파일이 없는 대상은 아래와 같습니다.</t>
     </r>
     <r>
       <rPr>
@@ -922,45 +727,13 @@
     <r>
       <rPr>
         <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{2}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
         <color rgb="FF00B050"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>확인하여 주시기 바랍니다.</t>
+      <t>확인요청드립니다.</t>
     </r>
     <r>
       <rPr>
@@ -976,13 +749,13 @@
     <r>
       <rPr>
         <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>감사합니다.</t>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{2}</t>
     </r>
     <r>
       <rPr>
@@ -1004,18 +777,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Link : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{3}</t>
+      <t>감사합니다.</t>
     </r>
     <r>
       <rPr>
@@ -1027,6 +789,12 @@
       </rPr>
       <t>&lt;/span&gt;&lt;/p&gt;</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}=검색 시작 날짜
+{1}=검색 종료 날짜
+{2}=결과 표</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1300,7 +1068,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1320,12 +1088,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1347,9 +1109,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1372,42 +1131,20 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1422,12 +1159,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1439,6 +1170,37 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1778,456 +1540,468 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.8125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="75.625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.78515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="75.640625" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" ht="30">
+      <c r="A4" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.600000000000001">
+      <c r="A9" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="41"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="42"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="44"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="45"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="37"/>
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="49" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="21"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:3" ht="26.25">
-      <c r="A4" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="21" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17.600000000000001">
+      <c r="A26" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="18"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="18"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B29" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="75">
+      <c r="A30" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="60">
+      <c r="A31" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="21"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="31"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="21" t="s">
+      <c r="C33" s="18"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="29" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="21"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="C37" s="39"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="29"/>
+      <c r="C38" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="39"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30">
+      <c r="A43" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="21" t="s">
+      <c r="B43" s="19"/>
+      <c r="C43" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="21"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="21" t="s">
+      <c r="B45" s="35"/>
+      <c r="C45" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" s="21"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
-    </row>
-    <row r="29" spans="1:3" ht="39.4">
-      <c r="A29" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="393.75">
-      <c r="A30" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="43" t="s">
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="52.5">
-      <c r="A31" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="43" t="s">
+      <c r="B46" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="35"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="21"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="45"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="44" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="45"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="46"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="47"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="26.25">
-      <c r="A43" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="48"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="48"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="48"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="48"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="48"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="48"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="48"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
+      <c r="A52" s="35"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="48"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
+      <c r="A53" s="35"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="48"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
+      <c r="A54" s="35"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="48"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
+      <c r="A55" s="35"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="48"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2243,6 +2017,10 @@
     <mergeCell ref="A20:B20"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1" xr:uid="{F03A4A92-A2C1-4CA7-AEA1-0669CE19F64A}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{155EAF24-B0EC-448E-9627-C31BCA88E509}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2255,11 +2033,11 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="49.75" style="4" customWidth="1"/>
-    <col min="3" max="3" width="100.9375" style="19" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.92578125" style="16" customWidth="1"/>
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -2270,330 +2048,330 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="14"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="C3" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23.15">
+      <c r="A4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="6">
         <v>5</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>97</v>
+      <c r="C4" s="12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="7">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="B5" s="9">
-        <v>5000</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="7">
+        <v>30000</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" s="9">
-        <v>30000</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7">
+        <v>120000</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" s="9">
-        <v>120000</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>48</v>
+      <c r="B9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="14"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B11" s="9">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="7">
+        <v>15000</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="B12" s="9">
-        <v>15000</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="7">
+        <v>60000</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" s="9">
-        <v>60000</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="14"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="14"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="9">
+        <v>99</v>
+      </c>
+      <c r="B25" s="7">
         <v>2</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>102</v>
+      <c r="C25" s="12" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="23.15">
+      <c r="A27" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="9">
-        <v>2</v>
-      </c>
-      <c r="C26" s="14" t="s">
+      <c r="B27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="14"/>
-    </row>
-    <row r="31" spans="1:3" ht="13.5">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="17"/>
-    </row>
-    <row r="32" spans="1:3" ht="13.5">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="1:3" ht="13.5">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="1:3" ht="13.5">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="17"/>
-    </row>
-    <row r="35" spans="1:3" ht="13.5">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="17"/>
-    </row>
-    <row r="36" spans="1:3" ht="13.5">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="17"/>
-    </row>
-    <row r="37" spans="1:3" ht="13.5">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="17"/>
-    </row>
-    <row r="38" spans="1:3" ht="13.5">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="17"/>
-    </row>
-    <row r="39" spans="1:3" ht="13.5">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="1:3" ht="13.5">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="18"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2609,14 +2387,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999"/>
+  <sheetFormatPr defaultRowHeight="17.600000000000001"/>
   <cols>
-    <col min="1" max="1" width="25.25" customWidth="1"/>
-    <col min="2" max="2" width="39.25" customWidth="1"/>
+    <col min="1" max="1" width="25.2109375" customWidth="1"/>
+    <col min="2" max="2" width="39.2109375" customWidth="1"/>
     <col min="3" max="3" width="98" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" thickBot="1">
+    <row r="1" spans="1:3" ht="18" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2624,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Config 파일 설정   • StartDate, EndDate 설정
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yache\Desktop\RPAWorkspace\RPA10_경기도뉴스포털_RE_노유정\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414709CC-B606-4B2F-BB71-ECF65782F6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7EB43E-4CC5-4AD3-8077-4204CA81528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -795,6 +795,26 @@
     <t>{0}=검색 시작 날짜
 {1}=검색 종료 날짜
 {2}=결과 표</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C:\RPA_Repository\ExPath\RPA10_Temp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartDate</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>EndDate</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>수신한 메일에서 추출한 시작날짜</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>수신한 메일에서 추출한 종료날짜</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1170,6 +1190,10 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1197,10 +1221,6 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1540,8 +1560,8 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1593,10 +1613,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="21" t="s">
         <v>6</v>
       </c>
@@ -1624,10 +1644,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="21" t="s">
         <v>11</v>
       </c>
@@ -1636,10 +1656,10 @@
       <c r="A9" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="42" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1648,21 +1668,21 @@
         <v>114</v>
       </c>
       <c r="B10" s="23"/>
-      <c r="C10" s="41"/>
+      <c r="C10" s="43"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="22" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="23"/>
-      <c r="C11" s="42"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="24" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="25"/>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1671,20 +1691,20 @@
         <v>15</v>
       </c>
       <c r="B13" s="26"/>
-      <c r="C13" s="44"/>
+      <c r="C13" s="46"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="45"/>
+      <c r="C14" s="47"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="37"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="21"/>
     </row>
     <row r="16" spans="1:3">
@@ -1715,17 +1735,17 @@
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="37"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="21"/>
     </row>
     <row r="21" spans="1:3">
@@ -1747,10 +1767,10 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="28" t="s">
         <v>83</v>
       </c>
@@ -1777,7 +1797,7 @@
       <c r="A26" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="37" t="s">
         <v>124</v>
       </c>
       <c r="C26" s="18"/>
@@ -1832,10 +1852,10 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="37"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="21"/>
     </row>
     <row r="33" spans="1:3">
@@ -1872,7 +1892,7 @@
         <v>79</v>
       </c>
       <c r="B36" s="29"/>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="40" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1883,14 +1903,14 @@
       <c r="B37" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="39"/>
+      <c r="C37" s="41"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="29"/>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="40" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1901,7 +1921,7 @@
       <c r="B39" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="39"/>
+      <c r="C39" s="41"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="33"/>
@@ -1956,15 +1976,23 @@
         <v>127</v>
       </c>
       <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
+      <c r="C47" s="35" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="35"/>
+      <c r="A48" s="35" t="s">
+        <v>135</v>
+      </c>
       <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
+      <c r="C48" s="35" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="35"/>
+      <c r="A49" s="35" t="s">
+        <v>136</v>
+      </c>
       <c r="B49" s="35"/>
       <c r="C49" s="35"/>
     </row>

</xml_diff>

<commit_message>
- Config 파일 설정   • UserAgent 값 설정 (HttpClient 요청용)   • ZipFileName 포맷 문자열 설정   • TotalCount 등 결과 저장용 항목 구성
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yache\Desktop\RPAWorkspace\RPA10_경기도뉴스포털_RE_노유정\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7EB43E-4CC5-4AD3-8077-4204CA81528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FBA3C3-B6DB-4B20-B473-AF161A4FA7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>CCTo</t>
-  </si>
-  <si>
-    <t>MailBody</t>
-  </si>
-  <si>
-    <t>MailBody_NoData</t>
   </si>
   <si>
     <t>File</t>
@@ -321,13 +315,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>{0}=날짜
-{1}=과제명 dicConfig("과제명").ToString
-{2}=기준정보시트 &amp; 다운로드대상시트 &amp; 20.다운로드대상폴더
-{3}=기준정보시트ID &amp; 다운로드대상시트ID &amp; 20.다운로드대상폴더ID</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>OrchestratorQueueFolder</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -434,6 +421,77 @@
   <si>
     <t>minasong621@gmail.com</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Today</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>yyyyMMdd 형식</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>yacheku@gmail.com</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>RPA10_경기도뉴스포털_RE_노유정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutputFolder</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>OutputPath</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Data\Output</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>{0} 첨부파일에 hwpx 파일 부재 알립니다.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}=yyyyMMdd(오늘날짜)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>{0}=검색 시작 날짜
+{1}=검색 종료 날짜
+{2}=결과 표</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C:\RPA_Repository\ExPath\RPA10_Temp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartDate</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>EndDate</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>수신한 메일에서 추출한 시작날짜</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>수신한 메일에서 추출한 종료날짜</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>TotalCount</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>{0}=검색 시작 날짜
+{1}=검색 종료 날짜</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -442,66 +500,13 @@
     <r>
       <rPr>
         <sz val="9"/>
-        <color rgb="FFFF0000"/>
+        <color theme="9"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RPA_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>결과 안내 메일입니다.</t>
+      <t>안녕하세요.</t>
     </r>
     <r>
       <rPr>
@@ -512,161 +517,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{2}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>확인하여 주시기 바랍니다.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>감사합니다.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Link : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{3}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;</t>
-    </r>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Today</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>yyyyMMdd 형식</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>yacheku@gmail.com</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>RPA10_경기도뉴스포털_RE_노유정</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>OutputFolder</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>OutputPath</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Data\Output</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://gnews.gg.go.kr/briefing/brief_gongbo.do</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>{0} 첨부파일에 hwpx 파일 부재 알립니다.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}=yyyyMMdd(오늘날짜)</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;안녕하세요.&lt;/span&gt;&lt;/p&gt;
 &lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
     </r>
     <r>
@@ -705,7 +555,7 @@
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
+        <color theme="9"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
@@ -792,29 +642,144 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>{0}=검색 시작 날짜
-{1}=검색 종료 날짜
-{2}=결과 표</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>C:\RPA_Repository\ExPath\RPA10_Temp</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>StartDate</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>EndDate</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>수신한 메일에서 추출한 시작날짜</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>수신한 메일에서 추출한 종료날짜</t>
+    <r>
+      <t>&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>안녕하세요.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ~ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>검색기간내에 hwpx 파일이 모두 존재합니다.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>감사합니다.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://gnews.gg.go.kr</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>MailBody</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>MailBody_NoData</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>UserAgent</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Safari/537.36</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ZipFileName</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>{0}_경기보도자료.zip</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -822,7 +787,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,6 +917,14 @@
     <font>
       <sz val="9"/>
       <color rgb="FF00B050"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="9"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1560,8 +1533,8 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1588,7 +1561,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C2" s="18"/>
     </row>
@@ -1597,19 +1570,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="30">
       <c r="A4" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1634,10 +1607,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>9</v>
@@ -1654,10 +1627,10 @@
     </row>
     <row r="9" spans="1:3" ht="17.600000000000001">
       <c r="A9" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>12</v>
@@ -1665,14 +1638,14 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="43"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="44"/>
@@ -1709,7 +1682,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -1718,11 +1691,11 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1735,7 +1708,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>20</v>
@@ -1750,7 +1723,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18" t="s">
@@ -1759,7 +1732,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18" t="s">
@@ -1772,7 +1745,7 @@
       </c>
       <c r="B23" s="39"/>
       <c r="C23" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1781,7 +1754,7 @@
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1790,24 +1763,24 @@
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.600000000000001">
       <c r="A26" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C27" s="18"/>
     </row>
@@ -1820,106 +1793,106 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="75">
       <c r="A30" s="18" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="60">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45">
       <c r="A31" s="18" t="s">
-        <v>29</v>
+        <v>139</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="39"/>
       <c r="C32" s="21"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" s="29"/>
       <c r="C36" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="41"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39" s="41"/>
     </row>
@@ -1930,22 +1903,22 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30">
       <c r="A43" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1955,60 +1928,70 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="35" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B45" s="35"/>
       <c r="C45" s="35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="35" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C46" s="35"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="35" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B47" s="35"/>
       <c r="C47" s="35" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="35" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B48" s="35"/>
       <c r="C48" s="35" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="35" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B49" s="35"/>
       <c r="C49" s="35"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="35"/>
+      <c r="A50" s="35" t="s">
+        <v>133</v>
+      </c>
       <c r="B50" s="35"/>
       <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="35"/>
-      <c r="B51" s="35"/>
+      <c r="A51" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>141</v>
+      </c>
       <c r="C51" s="35"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="35"/>
-      <c r="B52" s="35"/>
+      <c r="A52" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>143</v>
+      </c>
       <c r="C52" s="35"/>
     </row>
     <row r="53" spans="1:3">
@@ -2087,57 +2070,57 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="23.15">
       <c r="A4" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4" s="6">
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7">
         <v>5000</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7">
         <v>30000</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7">
         <v>120000</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2150,10 +2133,10 @@
         <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2163,35 +2146,35 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7">
         <v>1000</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="7">
         <v>15000</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7">
         <v>60000</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2201,35 +2184,35 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="7">
         <v>0.6</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="7">
         <v>0.8</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" s="7">
         <v>0.9</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2239,101 +2222,101 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B25" s="7">
         <v>2</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B26" s="7">
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="23.15">
       <c r="A27" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B27" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2430,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>